<commit_message>
Updated BOM with buffer components
</commit_message>
<xml_diff>
--- a/iC-MHM-Encoder-BOM.xlsx
+++ b/iC-MHM-Encoder-BOM.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="155">
   <si>
     <t>PCB:</t>
   </si>
@@ -198,7 +198,7 @@
     <t>478-9903-1-ND</t>
   </si>
   <si>
-    <t>C1</t>
+    <t xml:space="preserve">C1, C4</t>
   </si>
   <si>
     <t>https://datasheets.kyocera-avx.com/AutoMLCC.pdf</t>
@@ -267,7 +267,7 @@
     <t>RHM10KADCT-ND</t>
   </si>
   <si>
-    <t>R5</t>
+    <t xml:space="preserve">R5, R9, R10, R11</t>
   </si>
   <si>
     <t>https://fscdn.rohm.com/en/products/databook/datasheet/passive/resistor/chip_resistor/esr-e.pdf</t>
@@ -352,6 +352,24 @@
   </si>
   <si>
     <t>https://www.ichaus.de/MHM_datasheet_en</t>
+  </si>
+  <si>
+    <t>SN74LVC3G07QDCURQ1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Texas Instruments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IC BUFFER NON-INVERT 5.5V 8VSSOP</t>
+  </si>
+  <si>
+    <t>296-23710-1-ND</t>
+  </si>
+  <si>
+    <t>U5</t>
+  </si>
+  <si>
+    <t>https://www.ti.com/general/docs/suppproductinfo.tsp?distId=10&amp;gotoUrl=https%3A%2F%2Fwww.ti.com%2Flit%2Fgpn%2Fsn74lvc3g07-q1</t>
   </si>
   <si>
     <t xml:space="preserve">The 2023960607 is out of stock on digikey but is available on mouser:</t>
@@ -466,9 +484,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="160" formatCode="[$$-409]#,##0.00"/>
     <numFmt numFmtId="161" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="162" formatCode="\$#,##0.00_);[Red](\$#,##0.00)"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -517,7 +536,7 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="1" fillId="2" borderId="0" numFmtId="44" applyNumberFormat="1" applyFont="0" applyFill="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="160" xfId="0" applyNumberFormat="1"/>
     <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
@@ -528,9 +547,8 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="161" xfId="0" applyNumberFormat="1"/>
     <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="162" xfId="0" applyNumberFormat="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1257,7 +1275,7 @@
         <v>59</v>
       </c>
       <c r="E10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F10" t="s">
         <v>60</v>
@@ -1373,7 +1391,7 @@
         <v>82</v>
       </c>
       <c r="E14">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F14" t="s">
         <v>83</v>
@@ -1532,85 +1550,88 @@
       </c>
     </row>
     <row r="20" ht="14.25">
-      <c r="A20" s="7"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="I20" s="7"/>
-      <c r="J20" s="8"/>
+      <c r="B20" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="E20" s="8">
+        <v>1</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="G20" s="5">
+        <v>0.68000000000000005</v>
+      </c>
+      <c r="H20" s="9">
+        <v>0.68000000000000005</v>
+      </c>
+      <c r="I20" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="J20" s="8" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="21" ht="14.25">
-      <c r="A21" s="9" t="s">
+      <c r="A21" s="8"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="6"/>
+    </row>
+    <row r="22" ht="14.25">
+      <c r="A22" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B21" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="C21" s="10"/>
-      <c r="D21" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="E21" s="8"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="I21" s="7"/>
-      <c r="J21" s="8"/>
-    </row>
-    <row r="22" ht="14.25">
-      <c r="A22" s="7"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="I22" s="7"/>
-      <c r="J22" s="8"/>
+      <c r="B22" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="C22" s="8"/>
+      <c r="D22" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="E22" s="6"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="6"/>
     </row>
     <row r="23" ht="14.25">
-      <c r="A23" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="1"/>
-      <c r="I23" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="J23" s="8"/>
+      <c r="A23" s="8"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="6"/>
     </row>
     <row r="24" ht="14.25">
-      <c r="B24" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="C24" t="s">
-        <v>11</v>
-      </c>
-      <c r="D24" t="s">
-        <v>118</v>
-      </c>
-      <c r="E24">
-        <v>1</v>
-      </c>
-      <c r="F24" t="s">
-        <v>119</v>
-      </c>
-      <c r="G24" t="s">
-        <v>120</v>
-      </c>
-      <c r="H24" t="s">
+      <c r="A24" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="I24" t="s">
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="1"/>
+      <c r="I24" s="8" t="s">
         <v>122</v>
       </c>
+      <c r="J24" s="6"/>
     </row>
     <row r="25" ht="14.25">
-      <c r="B25" t="s">
+      <c r="B25" s="8" t="s">
         <v>123</v>
       </c>
       <c r="C25" t="s">
@@ -1672,7 +1693,7 @@
         <v>136</v>
       </c>
       <c r="E27">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="F27" t="s">
         <v>137</v>
@@ -1698,7 +1719,7 @@
         <v>142</v>
       </c>
       <c r="E28">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F28" t="s">
         <v>143</v>
@@ -1713,33 +1734,59 @@
         <v>146</v>
       </c>
     </row>
-    <row r="29" ht="14.25"/>
-    <row r="30" ht="14.25">
-      <c r="I30" s="12" t="s">
+    <row r="29" ht="14.25">
+      <c r="B29" t="s">
         <v>147</v>
       </c>
-    </row>
+      <c r="C29" t="s">
+        <v>11</v>
+      </c>
+      <c r="D29" t="s">
+        <v>148</v>
+      </c>
+      <c r="E29">
+        <v>20</v>
+      </c>
+      <c r="F29" t="s">
+        <v>149</v>
+      </c>
+      <c r="G29" t="s">
+        <v>150</v>
+      </c>
+      <c r="H29" t="s">
+        <v>151</v>
+      </c>
+      <c r="I29" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="30" ht="14.25"/>
     <row r="31" ht="14.25">
-      <c r="I31" s="12"/>
+      <c r="I31" s="11" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="32" ht="14.25">
-      <c r="I32" s="12"/>
+      <c r="I32" s="11"/>
     </row>
     <row r="33" ht="14.25">
-      <c r="I33" s="12"/>
+      <c r="I33" s="11"/>
     </row>
     <row r="34" ht="14.25">
-      <c r="I34" s="12"/>
+      <c r="I34" s="11"/>
     </row>
     <row r="35" ht="14.25">
-      <c r="I35" s="6" t="s">
-        <v>148</v>
+      <c r="I35" s="11"/>
+    </row>
+    <row r="36" ht="14.25">
+      <c r="I36" s="6" t="s">
+        <v>154</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="I30:I34"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="I31:I35"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="J2"/>
@@ -1761,8 +1808,9 @@
     <hyperlink r:id="rId17" ref="J18"/>
     <hyperlink r:id="rId18" ref="D19"/>
     <hyperlink r:id="rId19" ref="J19"/>
-    <hyperlink r:id="rId20" ref="D21"/>
-    <hyperlink r:id="rId21" ref="I35"/>
+    <hyperlink r:id="rId20" ref="J20"/>
+    <hyperlink r:id="rId21" ref="D22"/>
+    <hyperlink r:id="rId22" ref="I36"/>
   </hyperlinks>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>

</xml_diff>

<commit_message>
switched to 1k pullups and 0805 10uF
</commit_message>
<xml_diff>
--- a/iC-MHM-Encoder-BOM.xlsx
+++ b/iC-MHM-Encoder-BOM.xlsx
@@ -204,19 +204,22 @@
     <t>https://datasheets.kyocera-avx.com/AutoMLCC.pdf</t>
   </si>
   <si>
-    <t>0603ZD106KAT2A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAP CER 10UF 10V X5R 0603</t>
-  </si>
-  <si>
-    <t>478-10766-1-ND</t>
+    <t>CC0805MRX5R6BB106</t>
+  </si>
+  <si>
+    <t>YAGEO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAP CER 10UF 10V X5R 0805</t>
+  </si>
+  <si>
+    <t>311-3437-1-ND</t>
   </si>
   <si>
     <t xml:space="preserve">C2, C3</t>
   </si>
   <si>
-    <t>https://datasheets.kyocera-avx.com/cx5r.pdf</t>
+    <t>https://www.yageo.com/upload/media/product/productsearch/datasheet/mlcc/UPY-GPHC_X5R_4V-to-50V_26.pdf</t>
   </si>
   <si>
     <t>ERJ-PA3F1200V</t>
@@ -240,16 +243,13 @@
     <t>RE0603FRE071KL</t>
   </si>
   <si>
-    <t>YAGEO</t>
-  </si>
-  <si>
     <t xml:space="preserve">RES SMD 1K OHM 1% 1/10W 0603</t>
   </si>
   <si>
     <t>13-RE0603FRE071KLCT-ND</t>
   </si>
   <si>
-    <t xml:space="preserve">R7, R8</t>
+    <t xml:space="preserve">R7, R8, R9, R10, R11</t>
   </si>
   <si>
     <t>https://www.yageo.com/upload/media/product/productsearch/datasheet/rchip/PYu-RE_105_RoHS_L_6.pdf</t>
@@ -267,7 +267,7 @@
     <t>RHM10KADCT-ND</t>
   </si>
   <si>
-    <t xml:space="preserve">R5, R9, R10, R11</t>
+    <t>R5</t>
   </si>
   <si>
     <t>https://fscdn.rohm.com/en/products/databook/datasheet/passive/resistor/chip_resistor/esr-e.pdf</t>
@@ -536,7 +536,7 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="1" fillId="2" borderId="0" numFmtId="44" applyNumberFormat="1" applyFont="0" applyFill="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="160" xfId="0" applyNumberFormat="1"/>
     <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
@@ -545,11 +545,12 @@
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="161" xfId="1" applyNumberFormat="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="161" xfId="0" applyNumberFormat="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="162" xfId="0" applyNumberFormat="1"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1294,49 +1295,49 @@
       </c>
     </row>
     <row r="11">
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="6" t="s">
         <v>63</v>
       </c>
       <c r="C11" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="D11" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E11">
         <v>2</v>
       </c>
       <c r="F11" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G11" s="4">
-        <v>0.10000000000000001</v>
+        <v>0.20000000000000001</v>
       </c>
       <c r="H11" s="5">
-        <v>0.20000000000000001</v>
+        <v>0.40000000000000002</v>
       </c>
       <c r="I11" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="J11" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12">
       <c r="B12" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C12" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D12" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E12">
         <v>2</v>
       </c>
       <c r="F12" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G12" s="4">
         <v>0.14999999999999999</v>
@@ -1345,24 +1346,24 @@
         <v>0.29999999999999999</v>
       </c>
       <c r="I12" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="J12" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="13">
       <c r="B13" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C13" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="D13" t="s">
         <v>76</v>
       </c>
       <c r="E13">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F13" t="s">
         <v>77</v>
@@ -1371,7 +1372,7 @@
         <v>0.10000000000000001</v>
       </c>
       <c r="H13" s="5">
-        <v>0.20000000000000001</v>
+        <v>0.5</v>
       </c>
       <c r="I13" t="s">
         <v>78</v>
@@ -1391,7 +1392,7 @@
         <v>82</v>
       </c>
       <c r="E14">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F14" t="s">
         <v>83</v>
@@ -1414,7 +1415,7 @@
         <v>86</v>
       </c>
       <c r="C15" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D15" t="s">
         <v>87</v>
@@ -1443,7 +1444,7 @@
         <v>91</v>
       </c>
       <c r="C16" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="D16" t="s">
         <v>92</v>
@@ -1532,7 +1533,7 @@
       <c r="C19" t="s">
         <v>108</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D19" s="7" t="s">
         <v>109</v>
       </c>
       <c r="E19">
@@ -1545,12 +1546,12 @@
       <c r="I19" t="s">
         <v>111</v>
       </c>
-      <c r="J19" s="6" t="s">
+      <c r="J19" s="7" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="20" ht="14.25">
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="8" t="s">
         <v>113</v>
       </c>
       <c r="C20" s="8" t="s">
@@ -1571,7 +1572,7 @@
       <c r="H20" s="9">
         <v>0.68000000000000005</v>
       </c>
-      <c r="I20" s="10" t="s">
+      <c r="I20" s="8" t="s">
         <v>117</v>
       </c>
       <c r="J20" s="8" t="s">
@@ -1582,11 +1583,11 @@
       <c r="A21" s="8"/>
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
-      <c r="D21" s="6"/>
+      <c r="D21" s="7"/>
       <c r="E21" s="8"/>
       <c r="F21" s="8"/>
       <c r="I21" s="8"/>
-      <c r="J21" s="6"/>
+      <c r="J21" s="7"/>
     </row>
     <row r="22" ht="14.25">
       <c r="A22" s="2" t="s">
@@ -1596,24 +1597,24 @@
         <v>119</v>
       </c>
       <c r="C22" s="8"/>
-      <c r="D22" s="6" t="s">
+      <c r="D22" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="E22" s="6"/>
+      <c r="E22" s="7"/>
       <c r="F22" s="8"/>
       <c r="G22" s="8"/>
       <c r="I22" s="8"/>
-      <c r="J22" s="6"/>
+      <c r="J22" s="7"/>
     </row>
     <row r="23" ht="14.25">
       <c r="A23" s="8"/>
       <c r="B23" s="8"/>
       <c r="C23" s="8"/>
-      <c r="D23" s="6"/>
+      <c r="D23" s="7"/>
       <c r="E23" s="8"/>
       <c r="F23" s="8"/>
       <c r="I23" s="8"/>
-      <c r="J23" s="6"/>
+      <c r="J23" s="7"/>
     </row>
     <row r="24" ht="14.25">
       <c r="A24" s="8" t="s">
@@ -1621,14 +1622,14 @@
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>
-      <c r="D24" s="6"/>
+      <c r="D24" s="7"/>
       <c r="E24" s="8"/>
       <c r="F24" s="8"/>
       <c r="G24" s="1"/>
       <c r="I24" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="J24" s="6"/>
+      <c r="J24" s="7"/>
     </row>
     <row r="25" ht="14.25">
       <c r="B25" s="8" t="s">
@@ -1762,24 +1763,24 @@
     </row>
     <row r="30" ht="14.25"/>
     <row r="31" ht="14.25">
-      <c r="I31" s="11" t="s">
+      <c r="I31" s="10" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="32" ht="14.25">
-      <c r="I32" s="11"/>
+      <c r="I32" s="10"/>
     </row>
     <row r="33" ht="14.25">
-      <c r="I33" s="11"/>
+      <c r="I33" s="10"/>
     </row>
     <row r="34" ht="14.25">
-      <c r="I34" s="11"/>
+      <c r="I34" s="10"/>
     </row>
     <row r="35" ht="14.25">
-      <c r="I35" s="11"/>
+      <c r="I35" s="10"/>
     </row>
     <row r="36" ht="14.25">
-      <c r="I36" s="6" t="s">
+      <c r="I36" s="7" t="s">
         <v>154</v>
       </c>
     </row>
@@ -1798,19 +1799,18 @@
     <hyperlink r:id="rId7" ref="J8"/>
     <hyperlink r:id="rId8" ref="J9"/>
     <hyperlink r:id="rId9" ref="J10"/>
-    <hyperlink r:id="rId10" ref="J11"/>
-    <hyperlink r:id="rId11" ref="J12"/>
-    <hyperlink r:id="rId12" ref="J13"/>
-    <hyperlink r:id="rId13" ref="J14"/>
-    <hyperlink r:id="rId14" ref="J15"/>
-    <hyperlink r:id="rId15" ref="J16"/>
-    <hyperlink r:id="rId16" ref="J17"/>
-    <hyperlink r:id="rId17" ref="J18"/>
-    <hyperlink r:id="rId18" ref="D19"/>
-    <hyperlink r:id="rId19" ref="J19"/>
-    <hyperlink r:id="rId20" ref="J20"/>
-    <hyperlink r:id="rId21" ref="D22"/>
-    <hyperlink r:id="rId22" ref="I36"/>
+    <hyperlink r:id="rId10" ref="J12"/>
+    <hyperlink r:id="rId11" ref="J13"/>
+    <hyperlink r:id="rId12" ref="J14"/>
+    <hyperlink r:id="rId13" ref="J15"/>
+    <hyperlink r:id="rId14" ref="J16"/>
+    <hyperlink r:id="rId15" ref="J17"/>
+    <hyperlink r:id="rId16" ref="J18"/>
+    <hyperlink r:id="rId17" ref="D19"/>
+    <hyperlink r:id="rId18" ref="J19"/>
+    <hyperlink r:id="rId19" ref="J20"/>
+    <hyperlink r:id="rId20" ref="D22"/>
+    <hyperlink r:id="rId21" ref="I36"/>
   </hyperlinks>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>

</xml_diff>